<commit_message>
creacion workflow de modelos
</commit_message>
<xml_diff>
--- a/db_tandas/models_registry.xlsx
+++ b/db_tandas/models_registry.xlsx
@@ -5,15 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Universidad\Repositorios\P-Set2\db_tandas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge_j24fcle\OneDrive\Escritorio\repositorios\P-Set2\db_tandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9678270-387E-4F05-B163-C25D1000F2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC366740-AB6E-4185-B234-34F54766815A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Modelos" sheetId="1" r:id="rId1"/>
+    <sheet name="Ridge" sheetId="1" r:id="rId1"/>
+    <sheet name="Lasso" sheetId="3" r:id="rId2"/>
+    <sheet name="Elastic net" sheetId="2" r:id="rId3"/>
+    <sheet name="Arboles" sheetId="4" r:id="rId4"/>
+    <sheet name="Forest" sheetId="5" r:id="rId5"/>
+    <sheet name="Boosting" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>nombre resultados</t>
   </si>
@@ -53,9 +58,6 @@
     <t>tanda</t>
   </si>
   <si>
-    <t>MAE_training</t>
-  </si>
-  <si>
     <t>MAE_comp</t>
   </si>
   <si>
@@ -78,14 +80,31 @@
   </si>
   <si>
     <t>mixture</t>
+  </si>
+  <si>
+    <t>numero de modelo</t>
+  </si>
+  <si>
+    <t>tanda1_modelo1</t>
+  </si>
+  <si>
+    <t>test_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,9 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,78 +454,234 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="30.7265625" customWidth="1"/>
+    <col min="11" max="11" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>30.245804</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="1">
+      <c r="I2" s="1">
         <v>45210</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J3" s="1"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J4" s="1"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA81CDC-A987-4A1E-9ED2-D4335F948B07}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD93807B-CA29-4561-9944-C6DF81A0A8D9}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0F6C2-3AFA-41C2-B7E7-6C554E01DC08}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5B4A2-27DD-45E3-8CB5-626F3D8744BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86F0D8D-8478-4007-AE7A-CC5923F47E04}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hiper parametros en registro
</commit_message>
<xml_diff>
--- a/db_tandas/models_registry.xlsx
+++ b/db_tandas/models_registry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge_j24fcle\OneDrive\Escritorio\repositorios\P-Set2\db_tandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC366740-AB6E-4185-B234-34F54766815A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86965558-F673-4F25-BE0B-592EB54067E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ridge" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
   <si>
     <t>nombre resultados</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>test_1</t>
+  </si>
+  <si>
+    <t>tree_depth</t>
+  </si>
+  <si>
+    <t>min_n</t>
+  </si>
+  <si>
+    <t>mtry</t>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>learn_rate</t>
   </si>
 </sst>
 </file>
@@ -132,11 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36088E1E-5397-4A27-B5D2-BDB53431AEEB}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +526,7 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>30.245804</v>
+        <v>30245804</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -599,7 +613,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD93807B-CA29-4561-9944-C6DF81A0A8D9}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -642,46 +656,182 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E7" s="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0F6C2-3AFA-41C2-B7E7-6C554E01DC08}">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0F6C2-3AFA-41C2-B7E7-6C554E01DC08}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5B4A2-27DD-45E3-8CB5-626F3D8744BC}">
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5B4A2-27DD-45E3-8CB5-626F3D8744BC}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86F0D8D-8478-4007-AE7A-CC5923F47E04}">
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86F0D8D-8478-4007-AE7A-CC5923F47E04}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="13" max="13" width="21.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
archivos modelos y formato excel
</commit_message>
<xml_diff>
--- a/db_tandas/models_registry.xlsx
+++ b/db_tandas/models_registry.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge_j24fcle\OneDrive\Escritorio\repositorios\P-Set2\db_tandas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Universidad\Repositorios\P-Set2\db_tandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86965558-F673-4F25-BE0B-592EB54067E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D864D1DE-36B9-4EB1-B458-164EC5CF39C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{C564E30B-4F37-46F6-91C4-074D0E27D1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ridge" sheetId="1" r:id="rId1"/>
@@ -41,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
-  <si>
-    <t>nombre resultados</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
   <si>
     <t>Jorge</t>
   </si>
@@ -55,36 +52,12 @@
     <t>ridge</t>
   </si>
   <si>
-    <t>tanda</t>
-  </si>
-  <si>
     <t>MAE_comp</t>
   </si>
   <si>
     <t>Leaderboard</t>
   </si>
   <si>
-    <t>datos_usados</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>formula</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>submittor</t>
-  </si>
-  <si>
-    <t>mixture</t>
-  </si>
-  <si>
-    <t>numero de modelo</t>
-  </si>
-  <si>
     <t>tanda1_modelo1</t>
   </si>
   <si>
@@ -104,13 +77,43 @@
   </si>
   <si>
     <t>learn_rate</t>
+  </si>
+  <si>
+    <t>Nombre Resultados</t>
+  </si>
+  <si>
+    <t>Tanda</t>
+  </si>
+  <si>
+    <t>Datos_Usados</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Mixture</t>
+  </si>
+  <si>
+    <t>Especificación</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Submittor</t>
+  </si>
+  <si>
+    <t># De Modelo</t>
+  </si>
+  <si>
+    <t>Especificacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +129,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,10 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,65 +484,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36088E1E-5397-4A27-B5D2-BDB53431AEEB}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="8" max="8" width="30.7265625" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>30245804</v>
@@ -532,28 +552,28 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
         <v>45210</v>
       </c>
       <c r="J2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
     </row>
   </sheetData>
@@ -563,47 +583,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA81CDC-A987-4A1E-9ED2-D4335F948B07}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -613,47 +640,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD93807B-CA29-4561-9944-C6DF81A0A8D9}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -663,54 +704,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0F6C2-3AFA-41C2-B7E7-6C554E01DC08}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>13</v>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -720,56 +763,57 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5B4A2-27DD-45E3-8CB5-626F3D8744BC}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -779,56 +823,59 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86F0D8D-8478-4007-AE7A-CC5923F47E04}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>